<commit_message>
Lots of changes, graphing done
</commit_message>
<xml_diff>
--- a/All_Results.xlsx
+++ b/All_Results.xlsx
@@ -772,7 +772,7 @@
         <v>8019.703352289488</v>
       </c>
       <c r="D8" s="4" t="n">
-        <v>-6706.350945902536</v>
+        <v>6706.350945902536</v>
       </c>
       <c r="E8" s="6" t="n">
         <v>7139.905114274921</v>
@@ -812,7 +812,7 @@
         <v>7775.264560364717</v>
       </c>
       <c r="D9" s="4" t="n">
-        <v>-6950.789737827307</v>
+        <v>6950.789737827307</v>
       </c>
       <c r="E9" s="6" t="n">
         <v>7139.905114274921</v>
@@ -852,7 +852,7 @@
         <v>7601.581740812536</v>
       </c>
       <c r="D10" s="4" t="n">
-        <v>-7124.472557379489</v>
+        <v>7124.472557379489</v>
       </c>
       <c r="E10" s="6" t="n">
         <v>7139.905114274921</v>

</xml_diff>

<commit_message>
added more changes to graphing
</commit_message>
<xml_diff>
--- a/All_Results.xlsx
+++ b/All_Results.xlsx
@@ -588,55 +588,35 @@
       <c r="B5" s="4" t="n">
         <v>4.171</v>
       </c>
-      <c r="C5" s="8" t="inlineStr">
-        <is>
-          <t>OOR</t>
-        </is>
-      </c>
-      <c r="D5" s="8" t="inlineStr">
-        <is>
-          <t>OOR</t>
-        </is>
-      </c>
-      <c r="E5" s="6" t="inlineStr">
-        <is>
-          <t>OOR</t>
-        </is>
-      </c>
-      <c r="F5" s="6" t="inlineStr">
-        <is>
-          <t>OOR</t>
-        </is>
-      </c>
-      <c r="G5" s="8" t="inlineStr">
-        <is>
-          <t>OOR</t>
-        </is>
-      </c>
-      <c r="H5" s="8" t="inlineStr">
-        <is>
-          <t>OOR</t>
-        </is>
-      </c>
-      <c r="I5" s="6" t="inlineStr">
-        <is>
-          <t>OOR</t>
-        </is>
-      </c>
-      <c r="J5" s="8" t="inlineStr">
-        <is>
-          <t>OOR</t>
-        </is>
-      </c>
-      <c r="K5" s="8" t="inlineStr">
-        <is>
-          <t>OOR</t>
-        </is>
-      </c>
-      <c r="L5" s="8" t="inlineStr">
-        <is>
-          <t>OOR</t>
-        </is>
+      <c r="C5" s="8" t="n">
+        <v>5415.524044850007</v>
+      </c>
+      <c r="D5" s="8" t="n">
+        <v>3281.95083062353</v>
+      </c>
+      <c r="E5" s="6" t="n">
+        <v>1066.786607113238</v>
+      </c>
+      <c r="F5" s="6" t="n">
+        <v>1066.786607113238</v>
+      </c>
+      <c r="G5" s="8" t="n">
+        <v>56.76909753471365</v>
+      </c>
+      <c r="H5" s="8" t="n">
+        <v>13332.73375124685</v>
+      </c>
+      <c r="I5" s="6" t="n">
+        <v>983.5743079156682</v>
+      </c>
+      <c r="J5" s="8" t="n">
+        <v>533.4728362364156</v>
+      </c>
+      <c r="K5" s="8" t="n">
+        <v>196.196514182822</v>
+      </c>
+      <c r="L5" s="8" t="n">
+        <v>19361.86197272529</v>
       </c>
     </row>
     <row r="6" ht="18.75" customHeight="1">
@@ -648,55 +628,35 @@
       <c r="B6" s="4" t="n">
         <v>2.34</v>
       </c>
-      <c r="C6" s="8" t="inlineStr">
-        <is>
-          <t>OOR</t>
-        </is>
-      </c>
-      <c r="D6" s="8" t="inlineStr">
-        <is>
-          <t>OOR</t>
-        </is>
-      </c>
-      <c r="E6" s="6" t="inlineStr">
-        <is>
-          <t>OOR</t>
-        </is>
-      </c>
-      <c r="F6" s="6" t="inlineStr">
-        <is>
-          <t>OOR</t>
-        </is>
-      </c>
-      <c r="G6" s="8" t="inlineStr">
-        <is>
-          <t>OOR</t>
-        </is>
-      </c>
-      <c r="H6" s="8" t="inlineStr">
-        <is>
-          <t>OOR</t>
-        </is>
-      </c>
-      <c r="I6" s="6" t="inlineStr">
-        <is>
-          <t>OOR</t>
-        </is>
-      </c>
-      <c r="J6" s="8" t="inlineStr">
-        <is>
-          <t>OOR</t>
-        </is>
-      </c>
-      <c r="K6" s="8" t="inlineStr">
-        <is>
-          <t>OOR</t>
-        </is>
-      </c>
-      <c r="L6" s="8" t="inlineStr">
-        <is>
-          <t>OOR</t>
-        </is>
+      <c r="C6" s="8" t="n">
+        <v>1446.220395474019</v>
+      </c>
+      <c r="D6" s="8" t="n">
+        <v>687.3528187524578</v>
+      </c>
+      <c r="E6" s="6" t="n">
+        <v>1066.786607113238</v>
+      </c>
+      <c r="F6" s="6" t="n">
+        <v>1066.786607113238</v>
+      </c>
+      <c r="G6" s="8" t="n">
+        <v>0.9336061902159818</v>
+      </c>
+      <c r="H6" s="8" t="n">
+        <v>1186.664584156331</v>
+      </c>
+      <c r="I6" s="6" t="n">
+        <v>983.5743079156682</v>
+      </c>
+      <c r="J6" s="8" t="n">
+        <v>47.48113426565523</v>
+      </c>
+      <c r="K6" s="8" t="n">
+        <v>31.12607746882464</v>
+      </c>
+      <c r="L6" s="8" t="n">
+        <v>10862.32486602186</v>
       </c>
     </row>
     <row r="7" ht="18.75" customHeight="1">
@@ -708,55 +668,35 @@
       <c r="B7" s="4" t="n">
         <v>1.521</v>
       </c>
-      <c r="C7" s="8" t="inlineStr">
-        <is>
-          <t>OOR</t>
-        </is>
-      </c>
-      <c r="D7" s="8" t="inlineStr">
-        <is>
-          <t>OOR</t>
-        </is>
-      </c>
-      <c r="E7" s="6" t="inlineStr">
-        <is>
-          <t>OOR</t>
-        </is>
-      </c>
-      <c r="F7" s="6" t="inlineStr">
-        <is>
-          <t>OOR</t>
-        </is>
-      </c>
-      <c r="G7" s="8" t="inlineStr">
-        <is>
-          <t>OOR</t>
-        </is>
-      </c>
-      <c r="H7" s="8" t="inlineStr">
-        <is>
-          <t>OOR</t>
-        </is>
-      </c>
-      <c r="I7" s="6" t="inlineStr">
-        <is>
-          <t>OOR</t>
-        </is>
-      </c>
-      <c r="J7" s="8" t="inlineStr">
-        <is>
-          <t>OOR</t>
-        </is>
-      </c>
-      <c r="K7" s="8" t="inlineStr">
-        <is>
-          <t>OOR</t>
-        </is>
-      </c>
-      <c r="L7" s="8" t="inlineStr">
-        <is>
-          <t>OOR</t>
-        </is>
+      <c r="C7" s="8" t="n">
+        <v>1294.570534682059</v>
+      </c>
+      <c r="D7" s="8" t="n">
+        <v>839.0026795444178</v>
+      </c>
+      <c r="E7" s="6" t="n">
+        <v>1066.786607113238</v>
+      </c>
+      <c r="F7" s="6" t="n">
+        <v>1066.786607113238</v>
+      </c>
+      <c r="G7" s="8" t="n">
+        <v>-1.199625539479206</v>
+      </c>
+      <c r="H7" s="8" t="n">
+        <v>722.6160101329336</v>
+      </c>
+      <c r="I7" s="6" t="n">
+        <v>983.5743079156682</v>
+      </c>
+      <c r="J7" s="8" t="n">
+        <v>28.9135011339597</v>
+      </c>
+      <c r="K7" s="8" t="n">
+        <v>29.16020922704595</v>
+      </c>
+      <c r="L7" s="8" t="n">
+        <v>7060.511162914206</v>
       </c>
     </row>
     <row r="8" ht="18.75" customHeight="1">
@@ -769,34 +709,34 @@
         <v>1.143</v>
       </c>
       <c r="C8" s="4" t="n">
-        <v>8019.703352289488</v>
+        <v>1215.30424107269</v>
       </c>
       <c r="D8" s="4" t="n">
-        <v>6706.350945902536</v>
+        <v>918.2689731537868</v>
       </c>
       <c r="E8" s="6" t="n">
-        <v>7139.905114274921</v>
+        <v>1066.786607113238</v>
       </c>
       <c r="F8" s="6" t="n">
-        <v>7586.149183917103</v>
+        <v>1066.786607113238</v>
       </c>
       <c r="G8" s="4" t="n">
-        <v>1.923833770379531</v>
+        <v>-2.314650451073491</v>
       </c>
       <c r="H8" s="4" t="n">
-        <v>3652.252947800911</v>
+        <v>480.0611516882645</v>
       </c>
       <c r="I8" s="6" t="n">
-        <v>763.7567598375965</v>
+        <v>983.5743079156682</v>
       </c>
       <c r="J8" s="4" t="n">
-        <v>144.6126633325211</v>
+        <v>19.20833258476407</v>
       </c>
       <c r="K8" s="4" t="n">
-        <v>186.5068603760058</v>
+        <v>25.77879439013542</v>
       </c>
       <c r="L8" s="4" t="n">
-        <v>5521.252507376894</v>
+        <v>5305.827915326061</v>
       </c>
     </row>
     <row r="9" ht="18.75" customHeight="1">
@@ -809,34 +749,34 @@
         <v>0.867</v>
       </c>
       <c r="C9" s="4" t="n">
-        <v>7775.264560364717</v>
+        <v>1172.594880786659</v>
       </c>
       <c r="D9" s="4" t="n">
-        <v>6950.789737827307</v>
+        <v>960.9783334398184</v>
       </c>
       <c r="E9" s="6" t="n">
-        <v>7139.905114274921</v>
+        <v>1066.786607113238</v>
       </c>
       <c r="F9" s="6" t="n">
-        <v>7586.149183917103</v>
+        <v>1066.786607113238</v>
       </c>
       <c r="G9" s="4" t="n">
-        <v>1.297037211698649</v>
+        <v>-2.915435457016446</v>
       </c>
       <c r="H9" s="4" t="n">
-        <v>2711.163598890543</v>
+        <v>349.3705092130081</v>
       </c>
       <c r="I9" s="6" t="n">
-        <v>763.7567598375965</v>
+        <v>983.5743079156682</v>
       </c>
       <c r="J9" s="4" t="n">
-        <v>107.3497904907753</v>
+        <v>13.97910435508354</v>
       </c>
       <c r="K9" s="4" t="n">
-        <v>182.522673224482</v>
+        <v>24.73314910841883</v>
       </c>
       <c r="L9" s="4" t="n">
-        <v>4188.036678823943</v>
+        <v>4024.630623436303</v>
       </c>
     </row>
     <row r="10" ht="18.75" customHeight="1">
@@ -849,34 +789,34 @@
         <v>0.6909999999999999</v>
       </c>
       <c r="C10" s="4" t="n">
-        <v>7601.581740812536</v>
+        <v>1151.309911825298</v>
       </c>
       <c r="D10" s="4" t="n">
-        <v>7124.472557379489</v>
+        <v>982.2633024011792</v>
       </c>
       <c r="E10" s="6" t="n">
-        <v>7139.905114274921</v>
+        <v>1066.786607113238</v>
       </c>
       <c r="F10" s="6" t="n">
-        <v>7586.149183917103</v>
+        <v>1066.786607113238</v>
       </c>
       <c r="G10" s="4" t="n">
-        <v>0.8516750302704086</v>
+        <v>-3.214847345143676</v>
       </c>
       <c r="H10" s="4" t="n">
-        <v>2042.484743614645</v>
+        <v>284.2385041912438</v>
       </c>
       <c r="I10" s="6" t="n">
-        <v>763.7567598375965</v>
+        <v>983.5743079156682</v>
       </c>
       <c r="J10" s="4" t="n">
-        <v>80.87313852891884</v>
+        <v>11.37302550456456</v>
       </c>
       <c r="K10" s="4" t="n">
-        <v>172.5285479948262</v>
+        <v>25.24742739549875</v>
       </c>
       <c r="L10" s="4" t="n">
-        <v>3337.870063514815</v>
+        <v>3207.635248897907</v>
       </c>
     </row>
     <row r="11" ht="18.75" customHeight="1">
@@ -940,7 +880,7 @@
         </is>
       </c>
       <c r="B14" s="4" t="n">
-        <v>2.31</v>
+        <v>1.53</v>
       </c>
       <c r="C14" s="8" t="n"/>
       <c r="D14" s="8" t="n"/>
@@ -960,7 +900,7 @@
         </is>
       </c>
       <c r="B15" s="4" t="n">
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
       <c r="C15" s="8" t="n"/>
       <c r="D15" s="8" t="n"/>
@@ -980,7 +920,7 @@
         </is>
       </c>
       <c r="B16" s="4" t="n">
-        <v>0.018</v>
+        <v>0.012</v>
       </c>
       <c r="C16" s="8" t="n"/>
       <c r="D16" s="8" t="n"/>
@@ -1000,7 +940,7 @@
         </is>
       </c>
       <c r="B17" s="4" t="n">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="C17" s="8" t="n"/>
       <c r="D17" s="8" t="n"/>
@@ -1020,7 +960,7 @@
         </is>
       </c>
       <c r="B18" s="5" t="n">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C18" s="8" t="n"/>
       <c r="D18" s="8" t="n"/>
@@ -1060,7 +1000,7 @@
         </is>
       </c>
       <c r="B20" s="5" t="n">
-        <v>14729</v>
+        <v>2134</v>
       </c>
       <c r="C20" s="8" t="n"/>
       <c r="D20" s="8" t="n"/>
@@ -1100,7 +1040,7 @@
         </is>
       </c>
       <c r="B22" s="4" t="n">
-        <v>3.46</v>
+        <v>3.5</v>
       </c>
       <c r="C22" s="8" t="n"/>
       <c r="D22" s="8" t="n"/>
@@ -1120,7 +1060,7 @@
         </is>
       </c>
       <c r="B23" s="4" t="n">
-        <v>1.12</v>
+        <v>0.765</v>
       </c>
       <c r="C23" s="8" t="n"/>
       <c r="D23" s="8" t="n"/>
@@ -1140,7 +1080,7 @@
         </is>
       </c>
       <c r="B24" s="4" t="n">
-        <v>0.4</v>
+        <v>1.81</v>
       </c>
       <c r="C24" s="8" t="n"/>
       <c r="D24" s="8" t="n"/>
@@ -1160,7 +1100,7 @@
         </is>
       </c>
       <c r="B25" s="4" t="n">
-        <v>1.08</v>
+        <v>1.07</v>
       </c>
       <c r="C25" s="8" t="n"/>
       <c r="D25" s="8" t="n"/>

</xml_diff>

<commit_message>
made results all be positive
</commit_message>
<xml_diff>
--- a/All_Results.xlsx
+++ b/All_Results.xlsx
@@ -588,35 +588,55 @@
       <c r="B5" s="4" t="n">
         <v>4.171</v>
       </c>
-      <c r="C5" s="8" t="n">
-        <v>5415.524044850007</v>
-      </c>
-      <c r="D5" s="8" t="n">
-        <v>3281.95083062353</v>
-      </c>
-      <c r="E5" s="6" t="n">
-        <v>1066.786607113238</v>
-      </c>
-      <c r="F5" s="6" t="n">
-        <v>1066.786607113238</v>
-      </c>
-      <c r="G5" s="8" t="n">
-        <v>56.76909753471365</v>
-      </c>
-      <c r="H5" s="8" t="n">
-        <v>13332.73375124685</v>
-      </c>
-      <c r="I5" s="6" t="n">
-        <v>983.5743079156682</v>
-      </c>
-      <c r="J5" s="8" t="n">
-        <v>533.4728362364156</v>
-      </c>
-      <c r="K5" s="8" t="n">
-        <v>196.196514182822</v>
-      </c>
-      <c r="L5" s="8" t="n">
-        <v>19361.86197272529</v>
+      <c r="C5" s="8" t="inlineStr">
+        <is>
+          <t>OOR</t>
+        </is>
+      </c>
+      <c r="D5" s="8" t="inlineStr">
+        <is>
+          <t>OOR</t>
+        </is>
+      </c>
+      <c r="E5" s="6" t="inlineStr">
+        <is>
+          <t>OOR</t>
+        </is>
+      </c>
+      <c r="F5" s="6" t="inlineStr">
+        <is>
+          <t>OOR</t>
+        </is>
+      </c>
+      <c r="G5" s="8" t="inlineStr">
+        <is>
+          <t>OOR</t>
+        </is>
+      </c>
+      <c r="H5" s="8" t="inlineStr">
+        <is>
+          <t>OOR</t>
+        </is>
+      </c>
+      <c r="I5" s="6" t="inlineStr">
+        <is>
+          <t>OOR</t>
+        </is>
+      </c>
+      <c r="J5" s="8" t="inlineStr">
+        <is>
+          <t>OOR</t>
+        </is>
+      </c>
+      <c r="K5" s="8" t="inlineStr">
+        <is>
+          <t>OOR</t>
+        </is>
+      </c>
+      <c r="L5" s="8" t="inlineStr">
+        <is>
+          <t>OOR</t>
+        </is>
       </c>
     </row>
     <row r="6" ht="18.75" customHeight="1">
@@ -628,35 +648,55 @@
       <c r="B6" s="4" t="n">
         <v>2.34</v>
       </c>
-      <c r="C6" s="8" t="n">
-        <v>1446.220395474019</v>
-      </c>
-      <c r="D6" s="8" t="n">
-        <v>687.3528187524578</v>
-      </c>
-      <c r="E6" s="6" t="n">
-        <v>1066.786607113238</v>
-      </c>
-      <c r="F6" s="6" t="n">
-        <v>1066.786607113238</v>
-      </c>
-      <c r="G6" s="8" t="n">
-        <v>0.9336061902159818</v>
-      </c>
-      <c r="H6" s="8" t="n">
-        <v>1186.664584156331</v>
-      </c>
-      <c r="I6" s="6" t="n">
-        <v>983.5743079156682</v>
-      </c>
-      <c r="J6" s="8" t="n">
-        <v>47.48113426565523</v>
-      </c>
-      <c r="K6" s="8" t="n">
-        <v>31.12607746882464</v>
-      </c>
-      <c r="L6" s="8" t="n">
-        <v>10862.32486602186</v>
+      <c r="C6" s="8" t="inlineStr">
+        <is>
+          <t>OOR</t>
+        </is>
+      </c>
+      <c r="D6" s="8" t="inlineStr">
+        <is>
+          <t>OOR</t>
+        </is>
+      </c>
+      <c r="E6" s="6" t="inlineStr">
+        <is>
+          <t>OOR</t>
+        </is>
+      </c>
+      <c r="F6" s="6" t="inlineStr">
+        <is>
+          <t>OOR</t>
+        </is>
+      </c>
+      <c r="G6" s="8" t="inlineStr">
+        <is>
+          <t>OOR</t>
+        </is>
+      </c>
+      <c r="H6" s="8" t="inlineStr">
+        <is>
+          <t>OOR</t>
+        </is>
+      </c>
+      <c r="I6" s="6" t="inlineStr">
+        <is>
+          <t>OOR</t>
+        </is>
+      </c>
+      <c r="J6" s="8" t="inlineStr">
+        <is>
+          <t>OOR</t>
+        </is>
+      </c>
+      <c r="K6" s="8" t="inlineStr">
+        <is>
+          <t>OOR</t>
+        </is>
+      </c>
+      <c r="L6" s="8" t="inlineStr">
+        <is>
+          <t>OOR</t>
+        </is>
       </c>
     </row>
     <row r="7" ht="18.75" customHeight="1">
@@ -668,35 +708,55 @@
       <c r="B7" s="4" t="n">
         <v>1.521</v>
       </c>
-      <c r="C7" s="8" t="n">
-        <v>1294.570534682059</v>
-      </c>
-      <c r="D7" s="8" t="n">
-        <v>839.0026795444178</v>
-      </c>
-      <c r="E7" s="6" t="n">
-        <v>1066.786607113238</v>
-      </c>
-      <c r="F7" s="6" t="n">
-        <v>1066.786607113238</v>
-      </c>
-      <c r="G7" s="8" t="n">
-        <v>-1.199625539479206</v>
-      </c>
-      <c r="H7" s="8" t="n">
-        <v>722.6160101329336</v>
-      </c>
-      <c r="I7" s="6" t="n">
-        <v>983.5743079156682</v>
-      </c>
-      <c r="J7" s="8" t="n">
-        <v>28.9135011339597</v>
-      </c>
-      <c r="K7" s="8" t="n">
-        <v>29.16020922704595</v>
-      </c>
-      <c r="L7" s="8" t="n">
-        <v>7060.511162914206</v>
+      <c r="C7" s="8" t="inlineStr">
+        <is>
+          <t>OOR</t>
+        </is>
+      </c>
+      <c r="D7" s="8" t="inlineStr">
+        <is>
+          <t>OOR</t>
+        </is>
+      </c>
+      <c r="E7" s="6" t="inlineStr">
+        <is>
+          <t>OOR</t>
+        </is>
+      </c>
+      <c r="F7" s="6" t="inlineStr">
+        <is>
+          <t>OOR</t>
+        </is>
+      </c>
+      <c r="G7" s="8" t="inlineStr">
+        <is>
+          <t>OOR</t>
+        </is>
+      </c>
+      <c r="H7" s="8" t="inlineStr">
+        <is>
+          <t>OOR</t>
+        </is>
+      </c>
+      <c r="I7" s="6" t="inlineStr">
+        <is>
+          <t>OOR</t>
+        </is>
+      </c>
+      <c r="J7" s="8" t="inlineStr">
+        <is>
+          <t>OOR</t>
+        </is>
+      </c>
+      <c r="K7" s="8" t="inlineStr">
+        <is>
+          <t>OOR</t>
+        </is>
+      </c>
+      <c r="L7" s="8" t="inlineStr">
+        <is>
+          <t>OOR</t>
+        </is>
       </c>
     </row>
     <row r="8" ht="18.75" customHeight="1">
@@ -709,34 +769,34 @@
         <v>1.143</v>
       </c>
       <c r="C8" s="4" t="n">
-        <v>1215.30424107269</v>
+        <v>8019.703352289488</v>
       </c>
       <c r="D8" s="4" t="n">
-        <v>918.2689731537868</v>
+        <v>6706.350945902536</v>
       </c>
       <c r="E8" s="6" t="n">
-        <v>1066.786607113238</v>
+        <v>7139.905114274921</v>
       </c>
       <c r="F8" s="6" t="n">
-        <v>1066.786607113238</v>
+        <v>7586.149183917103</v>
       </c>
       <c r="G8" s="4" t="n">
-        <v>-2.314650451073491</v>
+        <v>1.923833770379531</v>
       </c>
       <c r="H8" s="4" t="n">
-        <v>480.0611516882645</v>
+        <v>3652.252947800911</v>
       </c>
       <c r="I8" s="6" t="n">
-        <v>983.5743079156682</v>
+        <v>763.7567598375965</v>
       </c>
       <c r="J8" s="4" t="n">
-        <v>19.20833258476407</v>
+        <v>144.6126633325211</v>
       </c>
       <c r="K8" s="4" t="n">
-        <v>25.77879439013542</v>
+        <v>186.5068603760058</v>
       </c>
       <c r="L8" s="4" t="n">
-        <v>5305.827915326061</v>
+        <v>5521.252507376894</v>
       </c>
     </row>
     <row r="9" ht="18.75" customHeight="1">
@@ -749,34 +809,34 @@
         <v>0.867</v>
       </c>
       <c r="C9" s="4" t="n">
-        <v>1172.594880786659</v>
+        <v>7775.264560364717</v>
       </c>
       <c r="D9" s="4" t="n">
-        <v>960.9783334398184</v>
+        <v>6950.789737827307</v>
       </c>
       <c r="E9" s="6" t="n">
-        <v>1066.786607113238</v>
+        <v>7139.905114274921</v>
       </c>
       <c r="F9" s="6" t="n">
-        <v>1066.786607113238</v>
+        <v>7586.149183917103</v>
       </c>
       <c r="G9" s="4" t="n">
-        <v>-2.915435457016446</v>
+        <v>1.297037211698649</v>
       </c>
       <c r="H9" s="4" t="n">
-        <v>349.3705092130081</v>
+        <v>2711.163598890543</v>
       </c>
       <c r="I9" s="6" t="n">
-        <v>983.5743079156682</v>
+        <v>763.7567598375965</v>
       </c>
       <c r="J9" s="4" t="n">
-        <v>13.97910435508354</v>
+        <v>107.3497904907753</v>
       </c>
       <c r="K9" s="4" t="n">
-        <v>24.73314910841883</v>
+        <v>182.522673224482</v>
       </c>
       <c r="L9" s="4" t="n">
-        <v>4024.630623436303</v>
+        <v>4188.036678823943</v>
       </c>
     </row>
     <row r="10" ht="18.75" customHeight="1">
@@ -789,34 +849,34 @@
         <v>0.6909999999999999</v>
       </c>
       <c r="C10" s="4" t="n">
-        <v>1151.309911825298</v>
+        <v>7601.581740812536</v>
       </c>
       <c r="D10" s="4" t="n">
-        <v>982.2633024011792</v>
+        <v>7124.472557379489</v>
       </c>
       <c r="E10" s="6" t="n">
-        <v>1066.786607113238</v>
+        <v>7139.905114274921</v>
       </c>
       <c r="F10" s="6" t="n">
-        <v>1066.786607113238</v>
+        <v>7586.149183917103</v>
       </c>
       <c r="G10" s="4" t="n">
-        <v>-3.214847345143676</v>
+        <v>0.8516750302704086</v>
       </c>
       <c r="H10" s="4" t="n">
-        <v>284.2385041912438</v>
+        <v>2042.484743614645</v>
       </c>
       <c r="I10" s="6" t="n">
-        <v>983.5743079156682</v>
+        <v>763.7567598375965</v>
       </c>
       <c r="J10" s="4" t="n">
-        <v>11.37302550456456</v>
+        <v>80.87313852891884</v>
       </c>
       <c r="K10" s="4" t="n">
-        <v>25.24742739549875</v>
+        <v>172.5285479948262</v>
       </c>
       <c r="L10" s="4" t="n">
-        <v>3207.635248897907</v>
+        <v>3337.870063514815</v>
       </c>
     </row>
     <row r="11" ht="18.75" customHeight="1">
@@ -880,7 +940,7 @@
         </is>
       </c>
       <c r="B14" s="4" t="n">
-        <v>1.53</v>
+        <v>2.31</v>
       </c>
       <c r="C14" s="8" t="n"/>
       <c r="D14" s="8" t="n"/>
@@ -900,7 +960,7 @@
         </is>
       </c>
       <c r="B15" s="4" t="n">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
       <c r="C15" s="8" t="n"/>
       <c r="D15" s="8" t="n"/>
@@ -920,7 +980,7 @@
         </is>
       </c>
       <c r="B16" s="4" t="n">
-        <v>0.012</v>
+        <v>0.018</v>
       </c>
       <c r="C16" s="8" t="n"/>
       <c r="D16" s="8" t="n"/>
@@ -940,7 +1000,7 @@
         </is>
       </c>
       <c r="B17" s="4" t="n">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="C17" s="8" t="n"/>
       <c r="D17" s="8" t="n"/>
@@ -960,7 +1020,7 @@
         </is>
       </c>
       <c r="B18" s="5" t="n">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C18" s="8" t="n"/>
       <c r="D18" s="8" t="n"/>
@@ -1000,7 +1060,7 @@
         </is>
       </c>
       <c r="B20" s="5" t="n">
-        <v>2134</v>
+        <v>14729</v>
       </c>
       <c r="C20" s="8" t="n"/>
       <c r="D20" s="8" t="n"/>
@@ -1040,7 +1100,7 @@
         </is>
       </c>
       <c r="B22" s="4" t="n">
-        <v>3.5</v>
+        <v>3.46</v>
       </c>
       <c r="C22" s="8" t="n"/>
       <c r="D22" s="8" t="n"/>
@@ -1060,7 +1120,7 @@
         </is>
       </c>
       <c r="B23" s="4" t="n">
-        <v>0.765</v>
+        <v>1.12</v>
       </c>
       <c r="C23" s="8" t="n"/>
       <c r="D23" s="8" t="n"/>
@@ -1080,7 +1140,7 @@
         </is>
       </c>
       <c r="B24" s="4" t="n">
-        <v>1.81</v>
+        <v>0.4</v>
       </c>
       <c r="C24" s="8" t="n"/>
       <c r="D24" s="8" t="n"/>
@@ -1100,7 +1160,7 @@
         </is>
       </c>
       <c r="B25" s="4" t="n">
-        <v>1.07</v>
+        <v>1.08</v>
       </c>
       <c r="C25" s="8" t="n"/>
       <c r="D25" s="8" t="n"/>

</xml_diff>